<commit_message>
Review all reports after CLT FAT, made some changes
Add 2 reports: 04.System Communication Behavior,   24. OSR Statistics
</commit_message>
<xml_diff>
--- a/development progress.xlsx
+++ b/development progress.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="90" windowWidth="19200" windowHeight="11640"/>
@@ -11,12 +11,12 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="62">
   <si>
     <t>id</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -158,66 +158,105 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Big Change</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>change</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>STD CAL</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>TO CBRA LINE</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>CHANGE</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>BASE ON ATR</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">NOT BASE ON </t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>BAG_INFO LOCATION_SEEN</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>BIG change</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ITEM_ENCODED, ADD MES</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Big change</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <t>FAT FIX</t>
+  </si>
+  <si>
+    <t>ALL SUBSYSTEM FROM ONE TABLE</t>
+  </si>
+  <si>
+    <t>ALL LOCATION FROM ONE TABLE</t>
+  </si>
+  <si>
+    <t>BAG_COUNT</t>
+  </si>
+  <si>
+    <t>IEC &amp; IRM</t>
+  </si>
+  <si>
+    <t>IEC.PLC_IDX&lt;&gt;'1001'</t>
+  </si>
+  <si>
+    <t>ITEM_ENCODED</t>
+  </si>
+  <si>
+    <t>0404/0405</t>
+  </si>
+  <si>
+    <t>ADD IRM</t>
+  </si>
+  <si>
+    <t>IRM LP</t>
+  </si>
+  <si>
+    <t>BRP &amp; BIT</t>
+  </si>
+  <si>
+    <t>ME LOCATION BASED ON MAINLINE</t>
+  </si>
+  <si>
+    <t>REMOVE DUPLICATE DATA</t>
+  </si>
+  <si>
+    <t>PRT_GET_FAULT_DURATION.sql</t>
+  </si>
+  <si>
+    <t>SHOW ALL CONV (NOT)
+ONLY TRACKING SUBSYSTEM</t>
+  </si>
+  <si>
+    <t>0407/0408</t>
+  </si>
+  <si>
+    <t>0409-NOW</t>
+  </si>
+  <si>
+    <t>OOG GID_USED</t>
+  </si>
+  <si>
+    <t>MDS_COUNT DIVERTER</t>
+  </si>
+  <si>
+    <t>REMOVE RPT_FORMAT_LOCATION</t>
+  </si>
+  <si>
+    <t>SUBSYSTEM BASED ON MIS_SubsystemCatalog</t>
+  </si>
+  <si>
+    <t>1.Remove EDS Location match
+2.Bag Cleared and Alarmed cal separately</t>
+  </si>
+  <si>
+    <t>Add ICR status for ITL</t>
+  </si>
+  <si>
+    <t>not sorted by PhotoCellID in template</t>
+  </si>
+  <si>
+    <t>1.Add max scan time</t>
+  </si>
+  <si>
+    <t>numeric value accuracy</t>
+  </si>
+  <si>
+    <t>correct second range(para)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="4">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -235,8 +274,14 @@
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -251,7 +296,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF00B0F0"/>
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -305,7 +362,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -330,9 +387,6 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
@@ -340,19 +394,57 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -426,6 +518,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -460,6 +553,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -635,27 +729,32 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A2:I30"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F11" sqref="F11"/>
+      <selection pane="bottomLeft" activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="8.875" style="6" customWidth="1"/>
-    <col min="2" max="2" width="43.875" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.25" style="3" customWidth="1"/>
-    <col min="4" max="4" width="24.625" style="3" customWidth="1"/>
+    <col min="1" max="1" width="8.85546875" style="6" customWidth="1"/>
+    <col min="2" max="2" width="43.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.28515625" style="3" customWidth="1"/>
+    <col min="4" max="4" width="24.5703125" style="3" customWidth="1"/>
     <col min="5" max="5" width="9" style="3"/>
-    <col min="6" max="6" width="10.125" style="9" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.125" customWidth="1"/>
+    <col min="6" max="6" width="21.42578125" style="8" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="36.140625" customWidth="1"/>
+    <col min="8" max="8" width="27.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:9">
+    <row r="1" spans="1:8">
+      <c r="F1" s="8" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
       <c r="A2" s="4" t="s">
         <v>0</v>
       </c>
@@ -671,12 +770,21 @@
       <c r="E2" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="3" spans="1:9">
+      <c r="F2" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="G2" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="H2" s="12" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="30">
       <c r="A3" s="5">
         <v>1</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="B3" s="15" t="s">
         <v>5</v>
       </c>
       <c r="C3" s="2" t="s">
@@ -686,26 +794,35 @@
         <v>33</v>
       </c>
       <c r="E3" s="2"/>
-      <c r="G3">
-        <v>20140321</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9">
+      <c r="F3" s="16" t="s">
+        <v>38</v>
+      </c>
+      <c r="H3" s="17" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
       <c r="A4" s="5">
         <v>2</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="7" t="s">
         <v>6</v>
       </c>
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
-    </row>
-    <row r="5" spans="1:9">
+      <c r="F4" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="H4" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
       <c r="A5" s="5">
         <v>3</v>
       </c>
-      <c r="B5" s="8" t="s">
+      <c r="B5" s="15" t="s">
         <v>7</v>
       </c>
       <c r="C5" s="2" t="s">
@@ -715,49 +832,35 @@
         <v>33</v>
       </c>
       <c r="E5" s="2"/>
-      <c r="G5">
-        <v>20140320</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9">
+    </row>
+    <row r="6" spans="1:8">
       <c r="A6" s="5">
         <v>4</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="15" t="s">
         <v>8</v>
       </c>
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
     </row>
-    <row r="7" spans="1:9">
+    <row r="7" spans="1:8">
       <c r="A7" s="5">
         <v>5</v>
       </c>
-      <c r="B7" s="8" t="s">
+      <c r="B7" s="15" t="s">
         <v>9</v>
       </c>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
-      <c r="F7" s="9" t="s">
-        <v>45</v>
-      </c>
-      <c r="G7">
-        <v>20140324</v>
-      </c>
-      <c r="H7" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="I7" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9">
+      <c r="H7" s="9"/>
+    </row>
+    <row r="8" spans="1:8">
       <c r="A8" s="5">
         <v>6</v>
       </c>
-      <c r="B8" s="8" t="s">
+      <c r="B8" s="15" t="s">
         <v>10</v>
       </c>
       <c r="C8" s="2" t="s">
@@ -767,18 +870,15 @@
         <v>34</v>
       </c>
       <c r="E8" s="2"/>
-      <c r="F8" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="G8">
-        <v>20140315</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9">
+      <c r="F8" s="16" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="45">
       <c r="A9" s="5">
         <v>7</v>
       </c>
-      <c r="B9" s="8" t="s">
+      <c r="B9" s="15" t="s">
         <v>11</v>
       </c>
       <c r="C9" s="2" t="s">
@@ -788,18 +888,18 @@
         <v>33</v>
       </c>
       <c r="E9" s="2"/>
-      <c r="F9" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="G9">
-        <v>20140320</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9">
+      <c r="F9" s="16" t="s">
+        <v>40</v>
+      </c>
+      <c r="G9" s="18" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8">
       <c r="A10" s="5">
         <v>8</v>
       </c>
-      <c r="B10" s="8" t="s">
+      <c r="B10" s="15" t="s">
         <v>12</v>
       </c>
       <c r="C10" s="2" t="s">
@@ -809,32 +909,32 @@
         <v>33</v>
       </c>
       <c r="E10" s="2"/>
-      <c r="F10" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="G10">
-        <v>20140324</v>
-      </c>
-      <c r="H10" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9">
+      <c r="F10" s="16" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8">
       <c r="A11" s="5">
         <v>9</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="B11" s="7" t="s">
         <v>13</v>
       </c>
       <c r="C11" s="2"/>
       <c r="D11" s="2"/>
       <c r="E11" s="2"/>
-    </row>
-    <row r="12" spans="1:9">
+      <c r="F11" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="H11" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8">
       <c r="A12" s="5">
         <v>10</v>
       </c>
-      <c r="B12" s="8" t="s">
+      <c r="B12" s="15" t="s">
         <v>14</v>
       </c>
       <c r="C12" s="2" t="s">
@@ -844,21 +944,16 @@
         <v>33</v>
       </c>
       <c r="E12" s="2"/>
-      <c r="F12" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="G12">
-        <v>20140320</v>
-      </c>
-      <c r="H12" s="11" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9">
+      <c r="G12" s="19" t="s">
+        <v>47</v>
+      </c>
+      <c r="H12" s="10"/>
+    </row>
+    <row r="13" spans="1:8">
       <c r="A13" s="5">
         <v>11</v>
       </c>
-      <c r="B13" s="8" t="s">
+      <c r="B13" s="15" t="s">
         <v>15</v>
       </c>
       <c r="C13" s="2" t="s">
@@ -868,11 +963,11 @@
         <v>33</v>
       </c>
       <c r="E13" s="2"/>
-      <c r="G13">
-        <v>20140321</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9">
+      <c r="F13" s="16" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8">
       <c r="A14" s="5">
         <v>12</v>
       </c>
@@ -883,7 +978,7 @@
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
     </row>
-    <row r="15" spans="1:9">
+    <row r="15" spans="1:8">
       <c r="A15" s="5">
         <v>13</v>
       </c>
@@ -894,11 +989,11 @@
       <c r="D15" s="2"/>
       <c r="E15" s="2"/>
     </row>
-    <row r="16" spans="1:9">
+    <row r="16" spans="1:8">
       <c r="A16" s="5">
         <v>14</v>
       </c>
-      <c r="B16" s="8" t="s">
+      <c r="B16" s="15" t="s">
         <v>18</v>
       </c>
       <c r="C16" s="2" t="s">
@@ -908,15 +1003,12 @@
         <v>33</v>
       </c>
       <c r="E16" s="2"/>
-      <c r="G16">
-        <v>20140319</v>
-      </c>
     </row>
     <row r="17" spans="1:8">
       <c r="A17" s="5">
         <v>15</v>
       </c>
-      <c r="B17" s="8" t="s">
+      <c r="B17" s="15" t="s">
         <v>19</v>
       </c>
       <c r="C17" s="2" t="s">
@@ -926,18 +1018,18 @@
         <v>34</v>
       </c>
       <c r="E17" s="2"/>
-      <c r="F17" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="G17">
-        <v>20140315</v>
+      <c r="F17" s="16" t="s">
+        <v>39</v>
+      </c>
+      <c r="G17" s="16" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="18" spans="1:8">
       <c r="A18" s="5">
         <v>16</v>
       </c>
-      <c r="B18" s="2" t="s">
+      <c r="B18" s="7" t="s">
         <v>20</v>
       </c>
       <c r="C18" s="2"/>
@@ -948,18 +1040,21 @@
       <c r="A19" s="5">
         <v>17</v>
       </c>
-      <c r="B19" s="2" t="s">
+      <c r="B19" s="7" t="s">
         <v>21</v>
       </c>
       <c r="C19" s="2"/>
       <c r="D19" s="2"/>
       <c r="E19" s="2"/>
+      <c r="H19" t="s">
+        <v>59</v>
+      </c>
     </row>
     <row r="20" spans="1:8">
       <c r="A20" s="5">
         <v>18</v>
       </c>
-      <c r="B20" s="8" t="s">
+      <c r="B20" s="15" t="s">
         <v>22</v>
       </c>
       <c r="C20" s="2" t="s">
@@ -969,14 +1064,14 @@
         <v>34</v>
       </c>
       <c r="E20" s="2"/>
-      <c r="F20" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="G20">
-        <v>20140320</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8">
+      <c r="G20" s="20" t="s">
+        <v>45</v>
+      </c>
+      <c r="H20" s="11" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" ht="60">
       <c r="A21" s="5">
         <v>19</v>
       </c>
@@ -986,12 +1081,15 @@
       <c r="C21" s="2"/>
       <c r="D21" s="2"/>
       <c r="E21" s="2"/>
+      <c r="H21" s="14" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="22" spans="1:8">
       <c r="A22" s="5">
         <v>20</v>
       </c>
-      <c r="B22" s="8" t="s">
+      <c r="B22" s="15" t="s">
         <v>24</v>
       </c>
       <c r="C22" s="2" t="s">
@@ -1001,21 +1099,15 @@
         <v>34</v>
       </c>
       <c r="E22" s="2"/>
-      <c r="F22" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="G22">
-        <v>20140319</v>
-      </c>
-      <c r="H22" s="11" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8">
+      <c r="H22" s="21" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" ht="30">
       <c r="A23" s="5">
         <v>21</v>
       </c>
-      <c r="B23" s="8" t="s">
+      <c r="B23" s="15" t="s">
         <v>25</v>
       </c>
       <c r="C23" s="2" t="s">
@@ -1025,15 +1117,21 @@
         <v>34</v>
       </c>
       <c r="E23" s="2"/>
-      <c r="G23">
-        <v>20140319</v>
+      <c r="F23" s="16" t="s">
+        <v>38</v>
+      </c>
+      <c r="G23" s="18" t="s">
+        <v>49</v>
+      </c>
+      <c r="H23" s="18" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="24" spans="1:8">
       <c r="A24" s="5">
         <v>22</v>
       </c>
-      <c r="B24" s="8" t="s">
+      <c r="B24" s="15" t="s">
         <v>26</v>
       </c>
       <c r="C24" s="2" t="s">
@@ -1043,15 +1141,12 @@
         <v>34</v>
       </c>
       <c r="E24" s="2"/>
-      <c r="G24">
-        <v>20140319</v>
-      </c>
     </row>
     <row r="25" spans="1:8">
       <c r="A25" s="5">
         <v>23</v>
       </c>
-      <c r="B25" s="8" t="s">
+      <c r="B25" s="15" t="s">
         <v>27</v>
       </c>
       <c r="C25" s="2" t="s">
@@ -1061,18 +1156,15 @@
         <v>33</v>
       </c>
       <c r="E25" s="2"/>
-      <c r="F25" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="G25">
-        <v>20140321</v>
+      <c r="H25" s="19" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="26" spans="1:8">
       <c r="A26" s="5">
         <v>24</v>
       </c>
-      <c r="B26" s="7" t="s">
+      <c r="B26" s="15" t="s">
         <v>28</v>
       </c>
       <c r="C26" s="2"/>
@@ -1083,7 +1175,7 @@
       <c r="A27" s="5">
         <v>25</v>
       </c>
-      <c r="B27" s="8" t="s">
+      <c r="B27" s="15" t="s">
         <v>29</v>
       </c>
       <c r="C27" s="2" t="s">
@@ -1093,15 +1185,15 @@
         <v>33</v>
       </c>
       <c r="E27" s="2"/>
-      <c r="G27">
-        <v>20140321</v>
+      <c r="F27" s="16" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="28" spans="1:8">
       <c r="A28" s="5">
         <v>26</v>
       </c>
-      <c r="B28" s="8" t="s">
+      <c r="B28" s="15" t="s">
         <v>30</v>
       </c>
       <c r="C28" s="2" t="s">
@@ -1111,21 +1203,12 @@
         <v>33</v>
       </c>
       <c r="E28" s="2"/>
-      <c r="F28" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="G28">
-        <v>20140324</v>
-      </c>
-      <c r="H28" t="s">
-        <v>42</v>
-      </c>
     </row>
     <row r="29" spans="1:8">
       <c r="A29" s="5">
         <v>27</v>
       </c>
-      <c r="B29" s="8" t="s">
+      <c r="B29" s="15" t="s">
         <v>31</v>
       </c>
       <c r="C29" s="2" t="s">
@@ -1137,18 +1220,18 @@
       <c r="E29" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="F29" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="G29">
-        <v>20140315</v>
+      <c r="F29" s="16" t="s">
+        <v>43</v>
+      </c>
+      <c r="G29" s="16" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="30" spans="1:8">
       <c r="A30" s="5">
         <v>28</v>
       </c>
-      <c r="B30" s="8" t="s">
+      <c r="B30" s="15" t="s">
         <v>32</v>
       </c>
       <c r="C30" s="2" t="s">
@@ -1158,8 +1241,25 @@
         <v>33</v>
       </c>
       <c r="E30" s="2"/>
-      <c r="G30">
-        <v>20140320</v>
+    </row>
+    <row r="33" spans="2:2">
+      <c r="B33" s="3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="34" spans="2:2">
+      <c r="B34" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="35" spans="2:2">
+      <c r="B35" s="3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="36" spans="2:2">
+      <c r="B36" s="13" t="s">
+        <v>54</v>
       </c>
     </row>
   </sheetData>
@@ -1170,12 +1270,12 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1184,12 +1284,12 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Add report 02, 09, 16, 17, 19 from CLT to OKC
</commit_message>
<xml_diff>
--- a/development progress.xlsx
+++ b/development progress.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="65">
   <si>
     <t>id</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -239,6 +239,15 @@
   </si>
   <si>
     <t>correct second range(para)</t>
+  </si>
+  <si>
+    <t>problem</t>
+  </si>
+  <si>
+    <t xml:space="preserve">new HSPD </t>
+  </si>
+  <si>
+    <t>EDS Flushes</t>
   </si>
 </sst>
 </file>
@@ -362,7 +371,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -384,9 +393,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
@@ -427,6 +433,15 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -730,11 +745,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H36"/>
+  <dimension ref="A1:I36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C15" sqref="C15"/>
+      <selection pane="bottomLeft" activeCell="B21" activeCellId="4" sqref="B4 B11 B18 B19 B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -744,17 +759,18 @@
     <col min="3" max="3" width="16.28515625" style="3" customWidth="1"/>
     <col min="4" max="4" width="24.5703125" style="3" customWidth="1"/>
     <col min="5" max="5" width="9" style="3"/>
-    <col min="6" max="6" width="21.42578125" style="8" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="36.140625" customWidth="1"/>
-    <col min="8" max="8" width="27.28515625" customWidth="1"/>
+    <col min="6" max="6" width="11.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="21.42578125" style="7" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="36.140625" customWidth="1"/>
+    <col min="9" max="9" width="27.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
-      <c r="F1" s="8" t="s">
+    <row r="1" spans="1:9">
+      <c r="G1" s="7" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:9">
       <c r="A2" s="4" t="s">
         <v>0</v>
       </c>
@@ -770,21 +786,24 @@
       <c r="E2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="8" t="s">
+      <c r="F2" s="21" t="s">
+        <v>62</v>
+      </c>
+      <c r="G2" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="G2" s="8" t="s">
+      <c r="H2" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="H2" s="12" t="s">
+      <c r="I2" s="11" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="30">
+    <row r="3" spans="1:9" ht="30">
       <c r="A3" s="5">
         <v>1</v>
       </c>
-      <c r="B3" s="15" t="s">
+      <c r="B3" s="14" t="s">
         <v>5</v>
       </c>
       <c r="C3" s="2" t="s">
@@ -794,35 +813,39 @@
         <v>33</v>
       </c>
       <c r="E3" s="2"/>
-      <c r="F3" s="16" t="s">
+      <c r="F3" s="22"/>
+      <c r="G3" s="15" t="s">
         <v>38</v>
       </c>
-      <c r="H3" s="17" t="s">
+      <c r="I3" s="16" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:9">
       <c r="A4" s="5">
         <v>2</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="14" t="s">
         <v>6</v>
       </c>
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
-      <c r="F4" s="8" t="s">
+      <c r="F4" s="23" t="s">
+        <v>63</v>
+      </c>
+      <c r="G4" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="H4" t="s">
+      <c r="I4" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:9">
       <c r="A5" s="5">
         <v>3</v>
       </c>
-      <c r="B5" s="15" t="s">
+      <c r="B5" s="14" t="s">
         <v>7</v>
       </c>
       <c r="C5" s="2" t="s">
@@ -832,35 +855,38 @@
         <v>33</v>
       </c>
       <c r="E5" s="2"/>
-    </row>
-    <row r="6" spans="1:8">
+      <c r="F5" s="22"/>
+    </row>
+    <row r="6" spans="1:9">
       <c r="A6" s="5">
         <v>4</v>
       </c>
-      <c r="B6" s="15" t="s">
+      <c r="B6" s="14" t="s">
         <v>8</v>
       </c>
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
-    </row>
-    <row r="7" spans="1:8">
+      <c r="F6" s="22"/>
+    </row>
+    <row r="7" spans="1:9">
       <c r="A7" s="5">
         <v>5</v>
       </c>
-      <c r="B7" s="15" t="s">
+      <c r="B7" s="14" t="s">
         <v>9</v>
       </c>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
-      <c r="H7" s="9"/>
-    </row>
-    <row r="8" spans="1:8">
+      <c r="F7" s="22"/>
+      <c r="I7" s="8"/>
+    </row>
+    <row r="8" spans="1:9">
       <c r="A8" s="5">
         <v>6</v>
       </c>
-      <c r="B8" s="15" t="s">
+      <c r="B8" s="14" t="s">
         <v>10</v>
       </c>
       <c r="C8" s="2" t="s">
@@ -870,15 +896,16 @@
         <v>34</v>
       </c>
       <c r="E8" s="2"/>
-      <c r="F8" s="16" t="s">
+      <c r="F8" s="22"/>
+      <c r="G8" s="15" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="45">
+    <row r="9" spans="1:9" ht="30">
       <c r="A9" s="5">
         <v>7</v>
       </c>
-      <c r="B9" s="15" t="s">
+      <c r="B9" s="14" t="s">
         <v>11</v>
       </c>
       <c r="C9" s="2" t="s">
@@ -888,18 +915,19 @@
         <v>33</v>
       </c>
       <c r="E9" s="2"/>
-      <c r="F9" s="16" t="s">
+      <c r="F9" s="22"/>
+      <c r="G9" s="15" t="s">
         <v>40</v>
       </c>
-      <c r="G9" s="18" t="s">
+      <c r="H9" s="17" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" spans="1:9">
       <c r="A10" s="5">
         <v>8</v>
       </c>
-      <c r="B10" s="15" t="s">
+      <c r="B10" s="14" t="s">
         <v>12</v>
       </c>
       <c r="C10" s="2" t="s">
@@ -909,32 +937,36 @@
         <v>33</v>
       </c>
       <c r="E10" s="2"/>
-      <c r="F10" s="16" t="s">
+      <c r="F10" s="22"/>
+      <c r="G10" s="15" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="11" spans="1:8">
+    <row r="11" spans="1:9">
       <c r="A11" s="5">
         <v>9</v>
       </c>
-      <c r="B11" s="7" t="s">
+      <c r="B11" s="14" t="s">
         <v>13</v>
       </c>
       <c r="C11" s="2"/>
       <c r="D11" s="2"/>
       <c r="E11" s="2"/>
-      <c r="F11" s="8" t="s">
+      <c r="F11" s="23" t="s">
+        <v>64</v>
+      </c>
+      <c r="G11" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="H11" t="s">
+      <c r="I11" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="12" spans="1:8">
+    <row r="12" spans="1:9">
       <c r="A12" s="5">
         <v>10</v>
       </c>
-      <c r="B12" s="15" t="s">
+      <c r="B12" s="14" t="s">
         <v>14</v>
       </c>
       <c r="C12" s="2" t="s">
@@ -944,16 +976,17 @@
         <v>33</v>
       </c>
       <c r="E12" s="2"/>
-      <c r="G12" s="19" t="s">
+      <c r="F12" s="22"/>
+      <c r="H12" s="18" t="s">
         <v>47</v>
       </c>
-      <c r="H12" s="10"/>
-    </row>
-    <row r="13" spans="1:8">
+      <c r="I12" s="9"/>
+    </row>
+    <row r="13" spans="1:9">
       <c r="A13" s="5">
         <v>11</v>
       </c>
-      <c r="B13" s="15" t="s">
+      <c r="B13" s="14" t="s">
         <v>15</v>
       </c>
       <c r="C13" s="2" t="s">
@@ -963,11 +996,12 @@
         <v>33</v>
       </c>
       <c r="E13" s="2"/>
-      <c r="F13" s="16" t="s">
+      <c r="F13" s="22"/>
+      <c r="G13" s="15" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="14" spans="1:8">
+    <row r="14" spans="1:9">
       <c r="A14" s="5">
         <v>12</v>
       </c>
@@ -977,8 +1011,9 @@
       <c r="C14" s="2"/>
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
-    </row>
-    <row r="15" spans="1:8">
+      <c r="F14" s="22"/>
+    </row>
+    <row r="15" spans="1:9">
       <c r="A15" s="5">
         <v>13</v>
       </c>
@@ -988,12 +1023,13 @@
       <c r="C15" s="2"/>
       <c r="D15" s="2"/>
       <c r="E15" s="2"/>
-    </row>
-    <row r="16" spans="1:8">
+      <c r="F15" s="22"/>
+    </row>
+    <row r="16" spans="1:9">
       <c r="A16" s="5">
         <v>14</v>
       </c>
-      <c r="B16" s="15" t="s">
+      <c r="B16" s="14" t="s">
         <v>18</v>
       </c>
       <c r="C16" s="2" t="s">
@@ -1003,12 +1039,13 @@
         <v>33</v>
       </c>
       <c r="E16" s="2"/>
-    </row>
-    <row r="17" spans="1:8">
+      <c r="F16" s="22"/>
+    </row>
+    <row r="17" spans="1:9">
       <c r="A17" s="5">
         <v>15</v>
       </c>
-      <c r="B17" s="15" t="s">
+      <c r="B17" s="14" t="s">
         <v>19</v>
       </c>
       <c r="C17" s="2" t="s">
@@ -1018,43 +1055,46 @@
         <v>34</v>
       </c>
       <c r="E17" s="2"/>
-      <c r="F17" s="16" t="s">
+      <c r="F17" s="22"/>
+      <c r="G17" s="15" t="s">
         <v>39</v>
       </c>
-      <c r="G17" s="16" t="s">
+      <c r="H17" s="15" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="18" spans="1:8">
+    <row r="18" spans="1:9">
       <c r="A18" s="5">
         <v>16</v>
       </c>
-      <c r="B18" s="7" t="s">
+      <c r="B18" s="14" t="s">
         <v>20</v>
       </c>
       <c r="C18" s="2"/>
       <c r="D18" s="2"/>
       <c r="E18" s="2"/>
-    </row>
-    <row r="19" spans="1:8">
+      <c r="F18" s="22"/>
+    </row>
+    <row r="19" spans="1:9">
       <c r="A19" s="5">
         <v>17</v>
       </c>
-      <c r="B19" s="7" t="s">
+      <c r="B19" s="14" t="s">
         <v>21</v>
       </c>
       <c r="C19" s="2"/>
       <c r="D19" s="2"/>
       <c r="E19" s="2"/>
-      <c r="H19" t="s">
+      <c r="F19" s="22"/>
+      <c r="I19" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="20" spans="1:8">
+    <row r="20" spans="1:9">
       <c r="A20" s="5">
         <v>18</v>
       </c>
-      <c r="B20" s="15" t="s">
+      <c r="B20" s="14" t="s">
         <v>22</v>
       </c>
       <c r="C20" s="2" t="s">
@@ -1064,32 +1104,34 @@
         <v>34</v>
       </c>
       <c r="E20" s="2"/>
-      <c r="G20" s="20" t="s">
+      <c r="F20" s="22"/>
+      <c r="H20" s="19" t="s">
         <v>45</v>
       </c>
-      <c r="H20" s="11" t="s">
+      <c r="I20" s="10" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="21" spans="1:8" ht="60">
+    <row r="21" spans="1:9" ht="60">
       <c r="A21" s="5">
         <v>19</v>
       </c>
-      <c r="B21" s="7" t="s">
+      <c r="B21" s="14" t="s">
         <v>23</v>
       </c>
       <c r="C21" s="2"/>
       <c r="D21" s="2"/>
       <c r="E21" s="2"/>
-      <c r="H21" s="14" t="s">
+      <c r="F21" s="22"/>
+      <c r="I21" s="13" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="22" spans="1:8">
+    <row r="22" spans="1:9">
       <c r="A22" s="5">
         <v>20</v>
       </c>
-      <c r="B22" s="15" t="s">
+      <c r="B22" s="14" t="s">
         <v>24</v>
       </c>
       <c r="C22" s="2" t="s">
@@ -1099,15 +1141,16 @@
         <v>34</v>
       </c>
       <c r="E22" s="2"/>
-      <c r="H22" s="21" t="s">
+      <c r="F22" s="22"/>
+      <c r="I22" s="20" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="23" spans="1:8" ht="30">
+    <row r="23" spans="1:9" ht="30">
       <c r="A23" s="5">
         <v>21</v>
       </c>
-      <c r="B23" s="15" t="s">
+      <c r="B23" s="14" t="s">
         <v>25</v>
       </c>
       <c r="C23" s="2" t="s">
@@ -1117,21 +1160,22 @@
         <v>34</v>
       </c>
       <c r="E23" s="2"/>
-      <c r="F23" s="16" t="s">
+      <c r="F23" s="22"/>
+      <c r="G23" s="15" t="s">
         <v>38</v>
       </c>
-      <c r="G23" s="18" t="s">
+      <c r="H23" s="17" t="s">
         <v>49</v>
       </c>
-      <c r="H23" s="18" t="s">
+      <c r="I23" s="17" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="24" spans="1:8">
+    <row r="24" spans="1:9">
       <c r="A24" s="5">
         <v>22</v>
       </c>
-      <c r="B24" s="15" t="s">
+      <c r="B24" s="14" t="s">
         <v>26</v>
       </c>
       <c r="C24" s="2" t="s">
@@ -1141,12 +1185,13 @@
         <v>34</v>
       </c>
       <c r="E24" s="2"/>
-    </row>
-    <row r="25" spans="1:8">
+      <c r="F24" s="22"/>
+    </row>
+    <row r="25" spans="1:9">
       <c r="A25" s="5">
         <v>23</v>
       </c>
-      <c r="B25" s="15" t="s">
+      <c r="B25" s="14" t="s">
         <v>27</v>
       </c>
       <c r="C25" s="2" t="s">
@@ -1156,26 +1201,28 @@
         <v>33</v>
       </c>
       <c r="E25" s="2"/>
-      <c r="H25" s="19" t="s">
+      <c r="F25" s="22"/>
+      <c r="I25" s="18" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="26" spans="1:8">
+    <row r="26" spans="1:9">
       <c r="A26" s="5">
         <v>24</v>
       </c>
-      <c r="B26" s="15" t="s">
+      <c r="B26" s="14" t="s">
         <v>28</v>
       </c>
       <c r="C26" s="2"/>
       <c r="D26" s="2"/>
       <c r="E26" s="2"/>
-    </row>
-    <row r="27" spans="1:8">
+      <c r="F26" s="22"/>
+    </row>
+    <row r="27" spans="1:9">
       <c r="A27" s="5">
         <v>25</v>
       </c>
-      <c r="B27" s="15" t="s">
+      <c r="B27" s="14" t="s">
         <v>29</v>
       </c>
       <c r="C27" s="2" t="s">
@@ -1185,15 +1232,16 @@
         <v>33</v>
       </c>
       <c r="E27" s="2"/>
-      <c r="F27" s="16" t="s">
+      <c r="F27" s="22"/>
+      <c r="G27" s="15" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="28" spans="1:8">
+    <row r="28" spans="1:9">
       <c r="A28" s="5">
         <v>26</v>
       </c>
-      <c r="B28" s="15" t="s">
+      <c r="B28" s="14" t="s">
         <v>30</v>
       </c>
       <c r="C28" s="2" t="s">
@@ -1203,12 +1251,13 @@
         <v>33</v>
       </c>
       <c r="E28" s="2"/>
-    </row>
-    <row r="29" spans="1:8">
+      <c r="F28" s="22"/>
+    </row>
+    <row r="29" spans="1:9">
       <c r="A29" s="5">
         <v>27</v>
       </c>
-      <c r="B29" s="15" t="s">
+      <c r="B29" s="14" t="s">
         <v>31</v>
       </c>
       <c r="C29" s="2" t="s">
@@ -1220,18 +1269,19 @@
       <c r="E29" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="F29" s="16" t="s">
+      <c r="F29" s="22"/>
+      <c r="G29" s="15" t="s">
         <v>43</v>
       </c>
-      <c r="G29" s="16" t="s">
+      <c r="H29" s="15" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="30" spans="1:8">
+    <row r="30" spans="1:9">
       <c r="A30" s="5">
         <v>28</v>
       </c>
-      <c r="B30" s="15" t="s">
+      <c r="B30" s="14" t="s">
         <v>32</v>
       </c>
       <c r="C30" s="2" t="s">
@@ -1241,6 +1291,7 @@
         <v>33</v>
       </c>
       <c r="E30" s="2"/>
+      <c r="F30" s="22"/>
     </row>
     <row r="33" spans="2:2">
       <c r="B33" s="3" t="s">
@@ -1258,7 +1309,7 @@
       </c>
     </row>
     <row r="36" spans="2:2">
-      <c r="B36" s="13" t="s">
+      <c r="B36" s="12" t="s">
         <v>54</v>
       </c>
     </row>

</xml_diff>